<commit_message>
Fixing the student save issue. and email uniqueness endpoints
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01-code\03-Work\01-SMS\application-service\src\test\resources\document\integration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="6"/>
   </bookViews>
@@ -366,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +400,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -479,6 +480,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -752,7 +754,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1901,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,12 +1923,12 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1976,52 +1978,56 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="12" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="12" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change end point path updated sheet
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01-code\03-Work\01-SMS\application-service\src\test\resources\document\integration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Audience" sheetId="3" r:id="rId1"/>
+    <sheet name="Audience-Completed" sheetId="3" r:id="rId1"/>
     <sheet name="Guardian" sheetId="19" r:id="rId2"/>
     <sheet name="Notification" sheetId="15" r:id="rId3"/>
     <sheet name="Notification Detail" sheetId="17" r:id="rId4"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="108">
   <si>
     <t>GET</t>
   </si>
@@ -141,9 +146,6 @@
     <t>/notifications/send</t>
   </si>
   <si>
-    <t>/notifications/update</t>
-  </si>
-  <si>
     <t>DELETED AS 1</t>
   </si>
   <si>
@@ -261,12 +263,6 @@
     <t>service not present</t>
   </si>
   <si>
-    <t>update is failing. Error has been shared in email</t>
-  </si>
-  <si>
-    <t>delete field not present. Make separate end point. We need to send email to user as well.</t>
-  </si>
-  <si>
     <t>UI issues</t>
   </si>
   <si>
@@ -331,6 +327,33 @@
   </si>
   <si>
     <t>13) Dashboard when data is not load fails. Please check email for details</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI </t>
+  </si>
+  <si>
+    <t>One minor issue of selection is still remaining which randomly appear</t>
+  </si>
+  <si>
+    <t>NOT WORKING</t>
+  </si>
+  <si>
+    <t>/notifications/delete/:id</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>14) notifications/delete/:id    return success but it doesn't delete base notification record</t>
+  </si>
+  <si>
+    <t>created: 09/10/2019</t>
+  </si>
+  <si>
+    <t>completed</t>
   </si>
 </sst>
 </file>
@@ -449,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -481,6 +504,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -754,7 +779,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,10 +788,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,6 +1008,16 @@
         <v>32</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -994,8 +1029,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1050,15 +1085,15 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
-        <v>33</v>
+      <c r="F3" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1066,7 +1101,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -1077,15 +1112,15 @@
         <v>33</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -1096,7 +1131,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,7 +1139,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1117,12 +1152,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>3</v>
@@ -1131,14 +1166,11 @@
         <v>19</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1152,19 +1184,16 @@
         <v>18</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>79</v>
+      <c r="F8" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -1177,10 +1206,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -1193,17 +1222,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1215,10 +1244,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,8 +1308,8 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
-        <v>33</v>
+      <c r="F3" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,36 +1346,20 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1391,12 +1404,12 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>34</v>
@@ -1422,7 +1435,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1474,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1477,7 +1490,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -1488,7 +1501,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1496,7 +1509,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1509,7 +1522,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1517,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -1530,7 +1543,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1538,7 +1551,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
@@ -1551,15 +1564,15 @@
         <v>33</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1620,10 +1633,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
@@ -1636,10 +1649,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -1652,10 +1665,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -1668,10 +1681,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
@@ -1684,10 +1697,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
@@ -1700,10 +1713,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>0</v>
@@ -1764,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1780,7 +1793,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -1796,7 +1809,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1814,7 +1827,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -1832,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
@@ -1847,10 +1860,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -1863,10 +1876,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1879,10 +1892,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -1901,139 +1914,151 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>101</v>
+      <c r="B29" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the rest endpoint sheets
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01-code\03-Work\01-SMS\application-service\src\test\resources\document\integration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Audience-Completed" sheetId="3" r:id="rId1"/>
@@ -21,7 +16,7 @@
     <sheet name="Session" sheetId="25" r:id="rId7"/>
     <sheet name="Munawar TODO List" sheetId="24" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
   <si>
     <t>GET</t>
   </si>
@@ -364,6 +359,9 @@
   </si>
   <si>
     <t>/employee/search/details/email/unique/:email/:id</t>
+  </si>
+  <si>
+    <t>Backend Status</t>
   </si>
 </sst>
 </file>
@@ -786,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1034,10 +1032,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,11 +1045,12 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1068,10 +1067,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1086,8 +1088,11 @@
       <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1100,10 +1105,13 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1115,14 +1123,17 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
@@ -1134,14 +1145,17 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1155,11 +1169,14 @@
         <v>30</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1176,8 +1193,11 @@
       <c r="F7" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1194,8 +1214,11 @@
       <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1207,11 +1230,14 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1223,21 +1249,24 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1439,10 +1468,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="A16:F16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,12 +1480,13 @@
     <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1473,10 +1503,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1491,8 +1524,11 @@
       <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1504,11 +1540,14 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1522,11 +1561,14 @@
         <v>30</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1540,11 +1582,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1558,11 +1603,14 @@
         <v>18</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
@@ -1574,11 +1622,14 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1590,11 +1641,14 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1606,11 +1660,14 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1622,11 +1679,14 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
@@ -1638,11 +1698,14 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
@@ -1654,11 +1717,14 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -1670,11 +1736,14 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1686,11 +1755,14 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -1702,11 +1774,14 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
@@ -1718,7 +1793,10 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1731,10 +1809,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,11 +1821,12 @@
     <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1764,10 +1843,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1779,11 +1861,14 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1795,11 +1880,14 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1813,11 +1901,14 @@
         <v>30</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1831,11 +1922,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1849,11 +1943,14 @@
         <v>18</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -1865,11 +1962,14 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>70</v>
       </c>
@@ -1881,11 +1981,14 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1900,8 +2003,11 @@
       <c r="F9" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>94</v>
       </c>
@@ -1913,7 +2019,10 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1939,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,47 +2079,47 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2069,7 +2178,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="11" t="s">
         <v>96</v>
       </c>
       <c r="B29" s="13" t="s">
@@ -2077,7 +2186,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C31" t="s">
@@ -2085,7 +2194,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C33" t="s">
@@ -2102,5 +2211,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
end point path details
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01-code\03-Work\01-SMS\application-service\src\test\resources\document\integration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Audience-Completed" sheetId="3" r:id="rId1"/>
@@ -13,8 +18,9 @@
     <sheet name="Notification Detail" sheetId="17" r:id="rId4"/>
     <sheet name="Student" sheetId="21" r:id="rId5"/>
     <sheet name="Employee" sheetId="23" r:id="rId6"/>
-    <sheet name="Session" sheetId="25" r:id="rId7"/>
-    <sheet name="Munawar TODO List" sheetId="24" r:id="rId8"/>
+    <sheet name="Create Session" sheetId="26" r:id="rId7"/>
+    <sheet name="Session" sheetId="25" r:id="rId8"/>
+    <sheet name="Munawar TODO List" sheetId="24" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="147">
   <si>
     <t>GET</t>
   </si>
@@ -362,6 +368,111 @@
   </si>
   <si>
     <t>Backend Status</t>
+  </si>
+  <si>
+    <t>list examtitles</t>
+  </si>
+  <si>
+    <t>list examtype</t>
+  </si>
+  <si>
+    <t>update examtitles</t>
+  </si>
+  <si>
+    <t>delete examtitles</t>
+  </si>
+  <si>
+    <t>update examtype</t>
+  </si>
+  <si>
+    <t>delete examtype</t>
+  </si>
+  <si>
+    <t>list sessioninfo</t>
+  </si>
+  <si>
+    <t>update sessioninfo</t>
+  </si>
+  <si>
+    <t>delete sessioninfo</t>
+  </si>
+  <si>
+    <t>list subject title</t>
+  </si>
+  <si>
+    <t>update subjects title</t>
+  </si>
+  <si>
+    <t>delete subjects title</t>
+  </si>
+  <si>
+    <t>list session subject</t>
+  </si>
+  <si>
+    <t>update session subject</t>
+  </si>
+  <si>
+    <t>delete session subject</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>step 1</t>
+  </si>
+  <si>
+    <t>step 2</t>
+  </si>
+  <si>
+    <t>step 3</t>
+  </si>
+  <si>
+    <t>list session exam</t>
+  </si>
+  <si>
+    <t>update session exam</t>
+  </si>
+  <si>
+    <t>delete session exam</t>
+  </si>
+  <si>
+    <t>save session exam</t>
+  </si>
+  <si>
+    <t>save examtitles</t>
+  </si>
+  <si>
+    <t>save examtype</t>
+  </si>
+  <si>
+    <t>save sessioninfo</t>
+  </si>
+  <si>
+    <t>save subject title</t>
+  </si>
+  <si>
+    <t>save session subject</t>
+  </si>
+  <si>
+    <t>step 4</t>
+  </si>
+  <si>
+    <t>list session test info</t>
+  </si>
+  <si>
+    <t>add session test info</t>
+  </si>
+  <si>
+    <t>delete session test info</t>
+  </si>
+  <si>
+    <t>update session test info</t>
+  </si>
+  <si>
+    <t>execute session</t>
+  </si>
+  <si>
+    <t>Step 5</t>
   </si>
 </sst>
 </file>
@@ -784,7 +895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2034,6 +2145,463 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2044,11 +2612,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
endpont changes of create session
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Audience-Completed" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="179">
   <si>
     <t>GET</t>
   </si>
@@ -388,15 +388,6 @@
     <t>delete examtype</t>
   </si>
   <si>
-    <t>list sessioninfo</t>
-  </si>
-  <si>
-    <t>update sessioninfo</t>
-  </si>
-  <si>
-    <t>delete sessioninfo</t>
-  </si>
-  <si>
     <t>list subject title</t>
   </si>
   <si>
@@ -445,9 +436,6 @@
     <t>save examtype</t>
   </si>
   <si>
-    <t>save sessioninfo</t>
-  </si>
-  <si>
     <t>save subject title</t>
   </si>
   <si>
@@ -473,6 +461,114 @@
   </si>
   <si>
     <t>Step 5</t>
+  </si>
+  <si>
+    <t>/examtitles/search/all</t>
+  </si>
+  <si>
+    <t>/examtypes/search/all</t>
+  </si>
+  <si>
+    <t>list active examtitles</t>
+  </si>
+  <si>
+    <t>/examtitles/search/all/active</t>
+  </si>
+  <si>
+    <t>list active examtype</t>
+  </si>
+  <si>
+    <t>/examtypes/search/all/active</t>
+  </si>
+  <si>
+    <t>/examtitles/save</t>
+  </si>
+  <si>
+    <t>/examtitles/update</t>
+  </si>
+  <si>
+    <t>/examtitles/delete/:id</t>
+  </si>
+  <si>
+    <t>/examtypes/save</t>
+  </si>
+  <si>
+    <t>/examtypes/update</t>
+  </si>
+  <si>
+    <t>/examtypes/delete/:id</t>
+  </si>
+  <si>
+    <t>save sessioninfo details</t>
+  </si>
+  <si>
+    <t>update sessioninfo details</t>
+  </si>
+  <si>
+    <t>delete sessioninfo details</t>
+  </si>
+  <si>
+    <t>details sessioninfo</t>
+  </si>
+  <si>
+    <t>/academicsession/search/details/:id</t>
+  </si>
+  <si>
+    <t>/academicsession/save</t>
+  </si>
+  <si>
+    <t>/academicsession/update</t>
+  </si>
+  <si>
+    <t>/academicsession/delete/:id</t>
+  </si>
+  <si>
+    <t>list active subject title</t>
+  </si>
+  <si>
+    <t>/subjecttitle/search/all/active</t>
+  </si>
+  <si>
+    <t>/subjecttitle/search/all</t>
+  </si>
+  <si>
+    <t>/subjecttitle/save</t>
+  </si>
+  <si>
+    <t>/subjecttitle/update</t>
+  </si>
+  <si>
+    <t>/subjecttitle/delete/:id</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>/academicsession/execute</t>
+  </si>
+  <si>
+    <t>unique examtitles</t>
+  </si>
+  <si>
+    <t>/examtitles/unique/name/:name/:id</t>
+  </si>
+  <si>
+    <t>unique examtype</t>
+  </si>
+  <si>
+    <t>/examtypes/unique/name/:name/:id</t>
+  </si>
+  <si>
+    <t>unique details sessioninfo name</t>
+  </si>
+  <si>
+    <t>/academicsession/unique/name/:name/:id</t>
+  </si>
+  <si>
+    <t>/subjecttitle/unique/name/:name/:id</t>
+  </si>
+  <si>
+    <t>unique details subject title name</t>
   </si>
 </sst>
 </file>
@@ -503,7 +599,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +647,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -591,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,6 +724,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -907,7 +1013,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1252,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,7 +1500,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1688,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +2029,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
@@ -2190,13 +2296,17 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2204,13 +2314,17 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2218,13 +2332,17 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2232,13 +2350,17 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2246,13 +2368,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2260,13 +2386,17 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2274,13 +2404,17 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2288,13 +2422,17 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2302,13 +2440,17 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2316,13 +2458,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2330,41 +2476,53 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2372,13 +2530,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2386,13 +2548,17 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -2400,13 +2566,17 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -2414,27 +2584,35 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2442,13 +2620,17 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2456,13 +2638,17 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2470,13 +2656,17 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2484,13 +2674,17 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2498,101 +2692,229 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="2" t="s">
+    <row r="25" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B30" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="7"/>
+      <c r="C37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EVL-150 Rest endpoints of ExamTitle and ExamType and removed some warnings
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01-code\03-Work\01-SMS\application-service\src\test\resources\document\integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Munawar\LaptopData\D_Drive\Munawar\work\StudentManagementSystem\application-service\src\test\resources\document\integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DBAC0E-4ACB-40B7-9575-5C2C8CD79074}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7755" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audience-Completed" sheetId="3" r:id="rId1"/>
@@ -22,17 +23,23 @@
     <sheet name="Session" sheetId="25" r:id="rId8"/>
     <sheet name="Munawar TODO List" sheetId="24" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="208">
   <si>
     <t>GET</t>
   </si>
@@ -490,18 +497,12 @@
     <t>/examtitles/update</t>
   </si>
   <si>
-    <t>/examtitles/delete/:id</t>
-  </si>
-  <si>
     <t>/examtypes/save</t>
   </si>
   <si>
     <t>/examtypes/update</t>
   </si>
   <si>
-    <t>/examtypes/delete/:id</t>
-  </si>
-  <si>
     <t>save sessioninfo details</t>
   </si>
   <si>
@@ -653,13 +654,66 @@
   </si>
   <si>
     <t>academicsession\02-examtype\details.json</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/examtitles/delete/:id  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/examtitles/update</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DELETE  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PUT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/examtypes/delete/:id  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/examtypes/update</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +730,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -777,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -812,6 +874,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1092,7 +1157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -1331,7 +1396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -1579,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1706,7 +1771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1767,7 +1832,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -2108,7 +2173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -2334,11 +2399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2420,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -2382,351 +2447,351 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="D10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="F14" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="D15" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="7"/>
@@ -2749,7 +2814,7 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="7"/>
@@ -2759,20 +2824,20 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="7"/>
@@ -2782,22 +2847,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="7"/>
@@ -2807,22 +2872,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="7"/>
@@ -2832,13 +2897,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>102</v>
@@ -2853,20 +2918,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="7"/>
@@ -2876,20 +2941,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="7"/>
@@ -2905,14 +2970,14 @@
         <v>128</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="7"/>
@@ -2928,16 +2993,16 @@
         <v>128</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="7"/>
@@ -2953,16 +3018,16 @@
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="7"/>
@@ -2978,7 +3043,7 @@
         <v>128</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>102</v>
@@ -2999,14 +3064,14 @@
         <v>143</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="7"/>
@@ -3019,7 +3084,7 @@
         <v>128</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -3035,7 +3100,7 @@
         <v>128</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -3051,7 +3116,7 @@
         <v>128</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -3067,7 +3132,7 @@
         <v>128</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -3083,7 +3148,7 @@
         <v>127</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
@@ -3099,7 +3164,7 @@
         <v>127</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
@@ -3115,7 +3180,7 @@
         <v>127</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
@@ -3131,7 +3196,7 @@
         <v>127</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
@@ -3147,7 +3212,7 @@
         <v>137</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
@@ -3163,7 +3228,7 @@
         <v>137</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -3179,7 +3244,7 @@
         <v>137</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
@@ -3195,7 +3260,7 @@
         <v>137</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -3210,7 +3275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3222,7 +3287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">

</xml_diff>

<commit_message>
EVL-150 Started creating session rest endpoint
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
+++ b/application-service/src/test/resources/document/integration/SMS-end-points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Munawar\LaptopData\D_Drive\Munawar\work\StudentManagementSystem\application-service\src\test\resources\document\integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DBAC0E-4ACB-40B7-9575-5C2C8CD79074}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DE821F-70FE-41A7-9260-070368A8EF84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,28 +2773,28 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="E16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">

</xml_diff>